<commit_message>
Added limits and several missed stations
</commit_message>
<xml_diff>
--- a/public/data/Lines.xlsx
+++ b/public/data/Lines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\web-projects\baltic-rails-leaflet\public\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{394A65F8-46EF-4911-A54B-DDB68109B4BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82E46183-C4A9-4935-AE2B-9A2D7F771608}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="99">
   <si>
     <t>Line ID</t>
   </si>
@@ -324,6 +324,12 @@
   </si>
   <si>
     <t>Liiva—Vääna</t>
+  </si>
+  <si>
+    <t>Tapa—Tartu—Koidula</t>
+  </si>
+  <si>
+    <t>Southern section rebuilt</t>
   </si>
 </sst>
 </file>
@@ -585,10 +591,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H53"/>
+  <dimension ref="A1:H54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="H53" sqref="H53"/>
+      <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1934,6 +1940,32 @@
         <v>0</v>
       </c>
     </row>
+    <row r="54" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
+        <v>109</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C54" s="1">
+        <v>1876</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F54" s="1">
+        <v>2011</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="H54" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>

</xml_diff>